<commit_message>
customer gross and country in groupby
</commit_message>
<xml_diff>
--- a/sofaaudit/output/Recoupable.xlsx
+++ b/sofaaudit/output/Recoupable.xlsx
@@ -3872,13 +3872,13 @@
         <v>184</v>
       </c>
       <c r="D145" s="3">
-        <v>-1895.95</v>
+        <v>-1895.94594594595</v>
       </c>
       <c r="E145" s="3">
-        <v>0</v>
+        <v>-935.44</v>
       </c>
       <c r="F145" s="3">
-        <v>-1895.95</v>
+        <v>-2831.38594594595</v>
       </c>
     </row>
     <row r="146" spans="1:6">

</xml_diff>

<commit_message>
merged audit and time ranges
</commit_message>
<xml_diff>
--- a/sofaaudit/output/Recoupable.xlsx
+++ b/sofaaudit/output/Recoupable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="326">
   <si>
     <t>Encoding U$</t>
   </si>
@@ -736,9 +736,6 @@
     <t>Feito gente grande</t>
   </si>
   <si>
-    <t>Gotitas de Alegria</t>
-  </si>
-  <si>
     <t>Helio Oiticica</t>
   </si>
   <si>
@@ -847,6 +844,27 @@
     <t>Violette</t>
   </si>
   <si>
+    <t>A Promisse</t>
+  </si>
+  <si>
+    <t>A walk with the tombstones</t>
+  </si>
+  <si>
+    <t>Dude where is my dog</t>
+  </si>
+  <si>
+    <t>Strech</t>
+  </si>
+  <si>
+    <t>Syngué sabour</t>
+  </si>
+  <si>
+    <t>Trinta</t>
+  </si>
+  <si>
+    <t>Une autre vie</t>
+  </si>
+  <si>
     <t>Tag Cultural</t>
   </si>
   <si>
@@ -859,9 +877,15 @@
     <t>Bromélia</t>
   </si>
   <si>
+    <t>Novelo</t>
+  </si>
+  <si>
     <t>Mares Filmes</t>
   </si>
   <si>
+    <t>Kinoscópio</t>
+  </si>
+  <si>
     <t>H2O INT</t>
   </si>
   <si>
@@ -871,12 +895,21 @@
     <t>H2O NAC</t>
   </si>
   <si>
+    <t>Escrevendo &amp; Filmes</t>
+  </si>
+  <si>
+    <t>Hangar Filmes</t>
+  </si>
+  <si>
     <t>Reserva Nacional</t>
   </si>
   <si>
     <t>Flash Star</t>
   </si>
   <si>
+    <t>TV Zero</t>
+  </si>
+  <si>
     <t>Vitrine</t>
   </si>
   <si>
@@ -892,25 +925,73 @@
     <t>Pandora</t>
   </si>
   <si>
+    <t>Autlook</t>
+  </si>
+  <si>
+    <t>Cinema 7</t>
+  </si>
+  <si>
     <t>Europa Filmes</t>
   </si>
   <si>
+    <t>Pequi Filmes</t>
+  </si>
+  <si>
     <t>Esfera</t>
   </si>
   <si>
+    <t>Oka Produções</t>
+  </si>
+  <si>
+    <t>RT Features</t>
+  </si>
+  <si>
+    <t>Maria Farinha</t>
+  </si>
+  <si>
+    <t>Coração da Selva</t>
+  </si>
+  <si>
+    <t>Cavídeo</t>
+  </si>
+  <si>
     <t>Alpha Filmes</t>
   </si>
   <si>
     <t>Alfhaville</t>
   </si>
   <si>
+    <t>Latam Distribution</t>
+  </si>
+  <si>
+    <t>Dama Filmes</t>
+  </si>
+  <si>
     <t>3 Film Group</t>
   </si>
   <si>
+    <t>Boulevard Filmes</t>
+  </si>
+  <si>
     <t>Nueva Era</t>
   </si>
   <si>
-    <t>Prodigo</t>
+    <t>Producciones Kramer</t>
+  </si>
+  <si>
+    <t>Guerrilha Filmes</t>
+  </si>
+  <si>
+    <t>Cinemascópio</t>
+  </si>
+  <si>
+    <t>Super Bebe</t>
+  </si>
+  <si>
+    <t>Jirafa</t>
+  </si>
+  <si>
+    <t>Primo Filmes</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F286"/>
+  <dimension ref="A1:F293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1309,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D2" s="3">
         <v>-924.01</v>
@@ -1329,7 +1410,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D3" s="3">
         <v>-692.28</v>
@@ -1349,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D4" s="3">
         <v>-1035</v>
@@ -1369,7 +1450,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D5" s="3">
         <v>-589.74</v>
@@ -1389,7 +1470,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D6" s="3">
         <v>-352.53</v>
@@ -1409,7 +1490,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D7" s="3">
         <v>-27.72</v>
@@ -1429,7 +1510,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D8" s="3">
         <v>-27.72</v>
@@ -1449,7 +1530,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D9" s="3">
         <v>-27.72</v>
@@ -1469,7 +1550,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D10" s="3">
         <v>-27.72</v>
@@ -1489,7 +1570,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D11" s="3">
         <v>-27.72</v>
@@ -1509,7 +1590,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D12" s="3">
         <v>-27.72</v>
@@ -1529,7 +1610,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D13" s="3">
         <v>-27.72</v>
@@ -1549,7 +1630,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D14" s="3">
         <v>-27.72</v>
@@ -1569,7 +1650,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D15" s="3">
         <v>-27.72</v>
@@ -1589,7 +1670,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D16" s="3">
         <v>-27.72</v>
@@ -1609,7 +1690,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D17" s="3">
         <v>-27.72</v>
@@ -1629,7 +1710,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D18" s="3">
         <v>-27.72</v>
@@ -1649,7 +1730,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D19" s="3">
         <v>-27.72</v>
@@ -1669,7 +1750,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D20" s="3">
         <v>-27.72</v>
@@ -1689,7 +1770,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D21" s="3">
         <v>-27.72</v>
@@ -1709,7 +1790,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D22" s="3">
         <v>-27.72</v>
@@ -1729,7 +1810,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D23" s="3">
         <v>-27.72</v>
@@ -1749,7 +1830,7 @@
         <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D24" s="3">
         <v>-27.72</v>
@@ -1769,7 +1850,7 @@
         <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D25" s="3">
         <v>-27.72</v>
@@ -1789,7 +1870,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D26" s="3">
         <v>-27.72</v>
@@ -1809,7 +1890,7 @@
         <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D27" s="3">
         <v>-27.72</v>
@@ -1829,7 +1910,7 @@
         <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D28" s="3">
         <v>-27.72</v>
@@ -1849,7 +1930,7 @@
         <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D29" s="3">
         <v>-27.72</v>
@@ -1869,7 +1950,7 @@
         <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D30" s="3">
         <v>-27.72</v>
@@ -1889,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D31" s="3">
         <v>-27.72</v>
@@ -1909,7 +1990,7 @@
         <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D32" s="3">
         <v>-27.72</v>
@@ -1929,7 +2010,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D33" s="3">
         <v>-27.72</v>
@@ -1949,7 +2030,7 @@
         <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D34" s="3">
         <v>-27.72</v>
@@ -1969,7 +2050,7 @@
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D35" s="3">
         <v>-27.72</v>
@@ -1989,7 +2070,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D36" s="3">
         <v>-27.72</v>
@@ -2009,7 +2090,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D37" s="3">
         <v>-27.72</v>
@@ -2029,7 +2110,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D38" s="3">
         <v>-27.72</v>
@@ -2049,7 +2130,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D39" s="3">
         <v>-27.72</v>
@@ -2069,7 +2150,7 @@
         <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D40" s="3">
         <v>-27.72</v>
@@ -2089,7 +2170,7 @@
         <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D41" s="3">
         <v>-27.72</v>
@@ -2109,7 +2190,7 @@
         <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D42" s="3">
         <v>-27.72</v>
@@ -2129,7 +2210,7 @@
         <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D43" s="3">
         <v>-27.72</v>
@@ -2149,7 +2230,7 @@
         <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D44" s="3">
         <v>-27.72</v>
@@ -2169,7 +2250,7 @@
         <v>49</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D45" s="3">
         <v>-27.72</v>
@@ -2189,7 +2270,7 @@
         <v>50</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D46" s="3">
         <v>-27.72</v>
@@ -2209,7 +2290,7 @@
         <v>51</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D47" s="3">
         <v>-27.72</v>
@@ -2229,7 +2310,7 @@
         <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D48" s="3">
         <v>-27.72</v>
@@ -2249,7 +2330,7 @@
         <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D49" s="3">
         <v>-857.92</v>
@@ -2269,7 +2350,7 @@
         <v>54</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D50" s="3">
         <v>-962.44</v>
@@ -2289,7 +2370,7 @@
         <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="D51" s="3">
         <v>-45.69</v>
@@ -2309,7 +2390,7 @@
         <v>56</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D52" s="3">
         <v>-25.03</v>
@@ -2329,7 +2410,7 @@
         <v>57</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D53" s="3">
         <v>-1035</v>
@@ -2349,7 +2430,7 @@
         <v>58</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D54" s="3">
         <v>-785.97</v>
@@ -2369,7 +2450,7 @@
         <v>59</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D55" s="3">
         <v>-692.28</v>
@@ -2389,7 +2470,7 @@
         <v>60</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="D56" s="3">
         <v>-589.74</v>
@@ -2409,7 +2490,7 @@
         <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D57" s="3">
         <v>-645.91</v>
@@ -2429,7 +2510,7 @@
         <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D58" s="3">
         <v>-308.91</v>
@@ -2449,7 +2530,7 @@
         <v>63</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D59" s="3">
         <v>-922.17</v>
@@ -2469,7 +2550,7 @@
         <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D60" s="3">
         <v>-308.91</v>
@@ -2489,7 +2570,7 @@
         <v>65</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D61" s="3">
         <v>-1106.57</v>
@@ -2509,7 +2590,7 @@
         <v>66</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D62" s="3">
         <v>-711.36</v>
@@ -2529,7 +2610,7 @@
         <v>67</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D63" s="3">
         <v>-1156.86</v>
@@ -2549,7 +2630,7 @@
         <v>68</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D64" s="3">
         <v>-228</v>
@@ -2569,7 +2650,7 @@
         <v>62</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D65" s="3">
         <v>-617.83</v>
@@ -2589,7 +2670,7 @@
         <v>69</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D66" s="3">
         <v>-1156.86</v>
@@ -2609,7 +2690,7 @@
         <v>70</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D67" s="3">
         <v>-887.77</v>
@@ -2629,7 +2710,7 @@
         <v>71</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D68" s="3">
         <v>-228</v>
@@ -2649,7 +2730,7 @@
         <v>72</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="D69" s="3">
         <v>-711.36</v>
@@ -2669,7 +2750,7 @@
         <v>73</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D70" s="3">
         <v>-645.91</v>
@@ -2689,7 +2770,7 @@
         <v>74</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D71" s="3">
         <v>-645.91</v>
@@ -2709,7 +2790,7 @@
         <v>75</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D72" s="3">
         <v>-664.09</v>
@@ -2729,7 +2810,7 @@
         <v>64</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D73" s="3">
         <v>-617.83</v>
@@ -2749,7 +2830,7 @@
         <v>76</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D74" s="3">
         <v>-645.91</v>
@@ -2769,7 +2850,7 @@
         <v>77</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D75" s="3">
         <v>-750</v>
@@ -2789,7 +2870,7 @@
         <v>78</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D76" s="3">
         <v>-609.99</v>
@@ -2809,7 +2890,7 @@
         <v>79</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="D77" s="3">
         <v>-623.64</v>
@@ -2829,7 +2910,7 @@
         <v>80</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D78" s="3">
         <v>-711.36</v>
@@ -2849,7 +2930,7 @@
         <v>81</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D79" s="3">
         <v>-557.55</v>
@@ -2869,7 +2950,7 @@
         <v>82</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D80" s="3">
         <v>-645.91</v>
@@ -2889,7 +2970,7 @@
         <v>83</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D81" s="3">
         <v>-737.64</v>
@@ -2909,7 +2990,7 @@
         <v>84</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="D82" s="3">
         <v>-1242</v>
@@ -2929,7 +3010,7 @@
         <v>85</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="D83" s="3">
         <v>-409.09</v>
@@ -2949,7 +3030,7 @@
         <v>86</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D84" s="3">
         <v>-751.14</v>
@@ -2969,7 +3050,7 @@
         <v>87</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D85" s="3">
         <v>-645.91</v>
@@ -2989,7 +3070,7 @@
         <v>88</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D86" s="3">
         <v>-1786.82</v>
@@ -3009,7 +3090,7 @@
         <v>89</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="D87" s="3">
         <v>-521.74</v>
@@ -3029,7 +3110,7 @@
         <v>90</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D88" s="3">
         <v>-711.13</v>
@@ -3049,7 +3130,7 @@
         <v>91</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="D89" s="3">
         <v>-391.3</v>
@@ -3069,7 +3150,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="D90" s="3">
         <v>-391.3</v>
@@ -3089,7 +3170,7 @@
         <v>93</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="D91" s="3">
         <v>-391.3</v>
@@ -3109,7 +3190,7 @@
         <v>94</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="D92" s="3">
         <v>-391.3</v>
@@ -3129,7 +3210,7 @@
         <v>95</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D93" s="3">
         <v>-696.52</v>
@@ -3149,7 +3230,7 @@
         <v>96</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="D94" s="3">
         <v>-478.26</v>
@@ -3169,7 +3250,7 @@
         <v>97</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="D95" s="3">
         <v>-391.3</v>
@@ -3189,7 +3270,7 @@
         <v>98</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D96" s="3">
         <v>-1865.65</v>
@@ -3209,7 +3290,7 @@
         <v>99</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D97" s="3">
         <v>-793.83</v>
@@ -3229,7 +3310,7 @@
         <v>100</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D98" s="3">
         <v>-617.83</v>
@@ -3249,7 +3330,7 @@
         <v>101</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D99" s="3">
         <v>-617.83</v>
@@ -3269,7 +3350,7 @@
         <v>102</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="D100" s="3">
         <v>-515.65</v>
@@ -3289,7 +3370,7 @@
         <v>103</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D101" s="3">
         <v>-2534.55</v>
@@ -3309,7 +3390,7 @@
         <v>104</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D102" s="3">
         <v>-519.99</v>
@@ -3329,7 +3410,7 @@
         <v>105</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D103" s="3">
         <v>-519.99</v>
@@ -3349,7 +3430,7 @@
         <v>106</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D104" s="3">
         <v>-787.77</v>
@@ -3369,7 +3450,7 @@
         <v>107</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D105" s="3">
         <v>-1916</v>
@@ -3389,7 +3470,7 @@
         <v>108</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D106" s="3">
         <v>-3149.5</v>
@@ -3409,7 +3490,7 @@
         <v>109</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="D107" s="3">
         <v>-272.73</v>
@@ -3429,7 +3510,7 @@
         <v>109</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="D108" s="3">
         <v>-545.45</v>
@@ -3449,7 +3530,7 @@
         <v>110</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D109" s="3">
         <v>-2102.27</v>
@@ -3469,7 +3550,7 @@
         <v>111</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D110" s="3">
         <v>-2075.82</v>
@@ -3489,7 +3570,7 @@
         <v>112</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D111" s="3">
         <v>-591.25</v>
@@ -3509,7 +3590,7 @@
         <v>113</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D112" s="3">
         <v>-631.36</v>
@@ -3529,7 +3610,7 @@
         <v>114</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D113" s="3">
         <v>-1849.27</v>
@@ -3549,7 +3630,7 @@
         <v>115</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D114" s="3">
         <v>-519.99</v>
@@ -3569,7 +3650,7 @@
         <v>116</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D115" s="3">
         <v>-631.36</v>
@@ -3589,7 +3670,7 @@
         <v>117</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D116" s="3">
         <v>-631.36</v>
@@ -3609,7 +3690,7 @@
         <v>118</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="D117" s="3">
         <v>-1203.41</v>
@@ -3629,7 +3710,7 @@
         <v>119</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D118" s="3">
         <v>-523.3</v>
@@ -3649,7 +3730,7 @@
         <v>120</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D119" s="3">
         <v>-631.36</v>
@@ -3669,7 +3750,7 @@
         <v>121</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="D120" s="3">
         <v>-333.18</v>
@@ -3689,7 +3770,7 @@
         <v>122</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D121" s="3">
         <v>-1914.14</v>
@@ -3709,7 +3790,7 @@
         <v>123</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D122" s="3">
         <v>-631.36</v>
@@ -3729,7 +3810,7 @@
         <v>124</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D123" s="3">
         <v>-625.68</v>
@@ -3749,7 +3830,7 @@
         <v>125</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D124" s="3">
         <v>-625.68</v>
@@ -3769,7 +3850,7 @@
         <v>126</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D125" s="3">
         <v>-625.68</v>
@@ -3789,7 +3870,7 @@
         <v>127</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D126" s="3">
         <v>-1859.14</v>
@@ -3809,7 +3890,7 @@
         <v>128</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D127" s="3">
         <v>-2086.04</v>
@@ -3829,7 +3910,7 @@
         <v>129</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D128" s="3">
         <v>-1859.14</v>
@@ -3849,7 +3930,7 @@
         <v>130</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D129" s="3">
         <v>-1704.5</v>
@@ -3869,7 +3950,7 @@
         <v>131</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D130" s="3">
         <v>-593.6</v>
@@ -3889,7 +3970,7 @@
         <v>132</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D131" s="3">
         <v>-1954.95</v>
@@ -3909,7 +3990,7 @@
         <v>133</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D132" s="3">
         <v>-1538.42</v>
@@ -3929,7 +4010,7 @@
         <v>134</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="D133" s="3">
         <v>-1531.53</v>
@@ -3949,7 +4030,7 @@
         <v>122</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D134" s="3">
         <v>-486.86</v>
@@ -3969,7 +4050,7 @@
         <v>135</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D135" s="3">
         <v>-625.68</v>
@@ -3989,7 +4070,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D136" s="3">
         <v>-1880.27</v>
@@ -4009,7 +4090,7 @@
         <v>137</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D137" s="3">
         <v>-625.68</v>
@@ -4029,7 +4110,7 @@
         <v>138</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D138" s="3">
         <v>-625.68</v>
@@ -4049,7 +4130,7 @@
         <v>139</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D139" s="3">
         <v>-615.87</v>
@@ -4069,7 +4150,7 @@
         <v>140</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="D140" s="3">
         <v>-630.63</v>
@@ -4089,7 +4170,7 @@
         <v>141</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D141" s="3">
         <v>-668.47</v>
@@ -4109,7 +4190,7 @@
         <v>142</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D142" s="3">
         <v>-1621.62</v>
@@ -4129,7 +4210,7 @@
         <v>143</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D143" s="3">
         <v>-1755.69</v>
@@ -4149,7 +4230,7 @@
         <v>144</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D144" s="3">
         <v>-1490.92</v>
@@ -4169,16 +4250,16 @@
         <v>145</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="D145" s="3">
-        <v>-1895.94594594595</v>
+        <v>-947.972972972973</v>
       </c>
       <c r="E145" s="3">
-        <v>-935.42</v>
+        <v>-467.72</v>
       </c>
       <c r="F145" s="3">
-        <v>-2831.36594594595</v>
+        <v>-1415.69297297297</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4186,19 +4267,19 @@
         <v>41791</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="D146" s="3">
-        <v>-625.68</v>
+        <v>-947.972972972973</v>
       </c>
       <c r="E146" s="3">
-        <v>0</v>
+        <v>-467.7</v>
       </c>
       <c r="F146" s="3">
-        <v>-625.68</v>
+        <v>-1415.67297297297</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -4206,10 +4287,10 @@
         <v>41791</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D147" s="3">
         <v>-625.68</v>
@@ -4226,30 +4307,30 @@
         <v>41791</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D148" s="3">
-        <v>-1950.9</v>
+        <v>-625.68</v>
       </c>
       <c r="E148" s="3">
         <v>0</v>
       </c>
       <c r="F148" s="3">
-        <v>-1950.9</v>
+        <v>-625.68</v>
       </c>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="2">
-        <v>41821</v>
+        <v>41791</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D149" s="3">
         <v>-1950.9</v>
@@ -4266,19 +4347,19 @@
         <v>41821</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="D150" s="3">
-        <v>-625.68</v>
+        <v>-1950.9</v>
       </c>
       <c r="E150" s="3">
         <v>0</v>
       </c>
       <c r="F150" s="3">
-        <v>-625.68</v>
+        <v>-1950.9</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -4286,19 +4367,19 @@
         <v>41821</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D151" s="3">
-        <v>-469.59</v>
+        <v>-625.68</v>
       </c>
       <c r="E151" s="3">
         <v>0</v>
       </c>
       <c r="F151" s="3">
-        <v>-469.59</v>
+        <v>-625.68</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -4306,19 +4387,19 @@
         <v>41821</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="D152" s="3">
-        <v>-1963.06306306306</v>
+        <v>-469.59</v>
       </c>
       <c r="E152" s="3">
         <v>0</v>
       </c>
       <c r="F152" s="3">
-        <v>-1963.06306306306</v>
+        <v>-469.59</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -4326,19 +4407,19 @@
         <v>41821</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="D153" s="3">
-        <v>-330.18</v>
+        <v>-1963.06306306306</v>
       </c>
       <c r="E153" s="3">
         <v>0</v>
       </c>
       <c r="F153" s="3">
-        <v>-330.18</v>
+        <v>-1963.06306306306</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4346,19 +4427,19 @@
         <v>41821</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="D154" s="3">
-        <v>-1951.53</v>
+        <v>-330.18</v>
       </c>
       <c r="E154" s="3">
         <v>0</v>
       </c>
       <c r="F154" s="3">
-        <v>-1951.53</v>
+        <v>-330.18</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4366,19 +4447,19 @@
         <v>41821</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D155" s="3">
-        <v>-1806.35</v>
+        <v>-1951.53</v>
       </c>
       <c r="E155" s="3">
         <v>0</v>
       </c>
       <c r="F155" s="3">
-        <v>-1806.35</v>
+        <v>-1951.53</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4386,19 +4467,19 @@
         <v>41821</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D156" s="3">
-        <v>-1951.53</v>
+        <v>-1806.35</v>
       </c>
       <c r="E156" s="3">
         <v>0</v>
       </c>
       <c r="F156" s="3">
-        <v>-1951.53</v>
+        <v>-1806.35</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -4406,19 +4487,19 @@
         <v>41821</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="D157" s="3">
-        <v>-1607.36</v>
+        <v>-1951.53</v>
       </c>
       <c r="E157" s="3">
         <v>0</v>
       </c>
       <c r="F157" s="3">
-        <v>-1607.36</v>
+        <v>-1951.53</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4426,19 +4507,19 @@
         <v>41821</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D158" s="3">
-        <v>-563.96</v>
+        <v>-1607.36</v>
       </c>
       <c r="E158" s="3">
         <v>0</v>
       </c>
       <c r="F158" s="3">
-        <v>-563.96</v>
+        <v>-1607.36</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4446,19 +4527,19 @@
         <v>41821</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D159" s="3">
-        <v>-540.54</v>
+        <v>-563.96</v>
       </c>
       <c r="E159" s="3">
         <v>0</v>
       </c>
       <c r="F159" s="3">
-        <v>-540.54</v>
+        <v>-563.96</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -4466,19 +4547,19 @@
         <v>41821</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>277</v>
+        <v>305</v>
       </c>
       <c r="D160" s="3">
-        <v>-2044.51</v>
+        <v>-540.54</v>
       </c>
       <c r="E160" s="3">
         <v>0</v>
       </c>
       <c r="F160" s="3">
-        <v>-2044.51</v>
+        <v>-540.54</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -4486,19 +4567,19 @@
         <v>41821</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D161" s="3">
-        <v>-625.675675675676</v>
+        <v>-2044.51</v>
       </c>
       <c r="E161" s="3">
         <v>0</v>
       </c>
       <c r="F161" s="3">
-        <v>-625.675675675676</v>
+        <v>-2044.51</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -4506,19 +4587,19 @@
         <v>41821</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>285</v>
       </c>
       <c r="D162" s="3">
-        <v>-552.43</v>
+        <v>-625.675675675676</v>
       </c>
       <c r="E162" s="3">
         <v>0</v>
       </c>
       <c r="F162" s="3">
-        <v>-552.43</v>
+        <v>-625.675675675676</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4526,19 +4607,19 @@
         <v>41821</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D163" s="3">
-        <v>-45.05</v>
+        <v>-552.43</v>
       </c>
       <c r="E163" s="3">
         <v>0</v>
       </c>
       <c r="F163" s="3">
-        <v>-45.05</v>
+        <v>-552.43</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4546,10 +4627,10 @@
         <v>41821</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D164" s="3">
         <v>-45.05</v>
@@ -4566,10 +4647,10 @@
         <v>41821</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D165" s="3">
         <v>-45.05</v>
@@ -4586,10 +4667,10 @@
         <v>41821</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D166" s="3">
         <v>-45.05</v>
@@ -4606,10 +4687,10 @@
         <v>41821</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D167" s="3">
         <v>-45.05</v>
@@ -4626,10 +4707,10 @@
         <v>41821</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D168" s="3">
         <v>-45.05</v>
@@ -4646,10 +4727,10 @@
         <v>41821</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D169" s="3">
         <v>-45.05</v>
@@ -4666,10 +4747,10 @@
         <v>41821</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D170" s="3">
         <v>-45.05</v>
@@ -4686,10 +4767,10 @@
         <v>41821</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D171" s="3">
         <v>-45.05</v>
@@ -4706,10 +4787,10 @@
         <v>41821</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D172" s="3">
         <v>-45.05</v>
@@ -4726,10 +4807,10 @@
         <v>41821</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D173" s="3">
         <v>-45.05</v>
@@ -4746,10 +4827,10 @@
         <v>41821</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D174" s="3">
         <v>-45.05</v>
@@ -4766,19 +4847,19 @@
         <v>41821</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="D175" s="3">
-        <v>-625.68</v>
+        <v>-45.05</v>
       </c>
       <c r="E175" s="3">
         <v>0</v>
       </c>
       <c r="F175" s="3">
-        <v>-625.68</v>
+        <v>-45.05</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -4786,39 +4867,39 @@
         <v>41821</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D176" s="3">
-        <v>-1577.20720720721</v>
+        <v>-625.68</v>
       </c>
       <c r="E176" s="3">
         <v>0</v>
       </c>
       <c r="F176" s="3">
-        <v>-1577.20720720721</v>
+        <v>-625.68</v>
       </c>
     </row>
     <row r="177" spans="1:6">
       <c r="A177" s="2">
-        <v>41852</v>
+        <v>41821</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D177" s="3">
-        <v>-6.51555555555556</v>
+        <v>-1577.20720720721</v>
       </c>
       <c r="E177" s="3">
         <v>0</v>
       </c>
       <c r="F177" s="3">
-        <v>-6.51555555555556</v>
+        <v>-1577.20720720721</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -4826,19 +4907,19 @@
         <v>41852</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D178" s="3">
-        <v>-1292.44444444444</v>
+        <v>-6.51555555555556</v>
       </c>
       <c r="E178" s="3">
         <v>0</v>
       </c>
       <c r="F178" s="3">
-        <v>-1292.44444444444</v>
+        <v>-6.51555555555556</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -4846,19 +4927,19 @@
         <v>41852</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D179" s="3">
-        <v>-1155.55555555556</v>
+        <v>-1292.44444444444</v>
       </c>
       <c r="E179" s="3">
         <v>0</v>
       </c>
       <c r="F179" s="3">
-        <v>-1155.55555555556</v>
+        <v>-1292.44444444444</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -4866,19 +4947,19 @@
         <v>41852</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="D180" s="3">
-        <v>-625.68</v>
+        <v>-1155.55555555556</v>
       </c>
       <c r="E180" s="3">
         <v>0</v>
       </c>
       <c r="F180" s="3">
-        <v>-625.68</v>
+        <v>-1155.55555555556</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -4886,19 +4967,19 @@
         <v>41852</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D181" s="3">
-        <v>-433.035555555556</v>
+        <v>-625.68</v>
       </c>
       <c r="E181" s="3">
         <v>0</v>
       </c>
       <c r="F181" s="3">
-        <v>-433.035555555556</v>
+        <v>-625.68</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -4906,19 +4987,19 @@
         <v>41852</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="D182" s="3">
-        <v>-1629.99</v>
+        <v>-433.035555555556</v>
       </c>
       <c r="E182" s="3">
         <v>0</v>
       </c>
       <c r="F182" s="3">
-        <v>-1629.99</v>
+        <v>-433.035555555556</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -4926,19 +5007,19 @@
         <v>41852</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="D183" s="3">
-        <v>-612.355555555555</v>
+        <v>-1629.99</v>
       </c>
       <c r="E183" s="3">
         <v>0</v>
       </c>
       <c r="F183" s="3">
-        <v>-612.355555555555</v>
+        <v>-1629.99</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -4946,19 +5027,19 @@
         <v>41852</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="D184" s="3">
-        <v>-1908.03555555556</v>
+        <v>-612.355555555555</v>
       </c>
       <c r="E184" s="3">
         <v>0</v>
       </c>
       <c r="F184" s="3">
-        <v>-1908.03555555556</v>
+        <v>-612.355555555555</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -4966,19 +5047,19 @@
         <v>41852</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>278</v>
+        <v>307</v>
       </c>
       <c r="D185" s="3">
-        <v>-335.404444444444</v>
+        <v>-1908.03555555556</v>
       </c>
       <c r="E185" s="3">
         <v>0</v>
       </c>
       <c r="F185" s="3">
-        <v>-335.404444444444</v>
+        <v>-1908.03555555556</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -4986,19 +5067,19 @@
         <v>41852</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
       <c r="D186" s="3">
-        <v>-405.41</v>
+        <v>-335.404444444444</v>
       </c>
       <c r="E186" s="3">
         <v>0</v>
       </c>
       <c r="F186" s="3">
-        <v>-405.41</v>
+        <v>-335.404444444444</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -5006,39 +5087,39 @@
         <v>41852</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="D187" s="3">
-        <v>-12.4444444444444</v>
+        <v>-408.293333333333</v>
       </c>
       <c r="E187" s="3">
         <v>0</v>
       </c>
       <c r="F187" s="3">
-        <v>-12.4444444444444</v>
+        <v>-408.293333333333</v>
       </c>
     </row>
     <row r="188" spans="1:6">
       <c r="A188" s="2">
-        <v>41883</v>
+        <v>41852</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="D188" s="3">
-        <v>-1992.44444444444</v>
+        <v>-12.4444444444444</v>
       </c>
       <c r="E188" s="3">
         <v>0</v>
       </c>
       <c r="F188" s="3">
-        <v>-1992.44444444444</v>
+        <v>-12.4444444444444</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -5046,19 +5127,19 @@
         <v>41883</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="D189" s="3">
-        <v>-1883.28888888889</v>
+        <v>-1992.44444444444</v>
       </c>
       <c r="E189" s="3">
         <v>0</v>
       </c>
       <c r="F189" s="3">
-        <v>-1883.28888888889</v>
+        <v>-1992.44444444444</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -5066,19 +5147,19 @@
         <v>41883</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D190" s="3">
-        <v>-44.4444444444444</v>
+        <v>-1883.28888888889</v>
       </c>
       <c r="E190" s="3">
         <v>0</v>
       </c>
       <c r="F190" s="3">
-        <v>-44.4444444444444</v>
+        <v>-1883.28888888889</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -5086,10 +5167,10 @@
         <v>41883</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D191" s="3">
         <v>-44.4444444444444</v>
@@ -5106,10 +5187,10 @@
         <v>41883</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D192" s="3">
         <v>-44.4444444444444</v>
@@ -5126,10 +5207,10 @@
         <v>41883</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D193" s="3">
         <v>-44.4444444444444</v>
@@ -5146,10 +5227,10 @@
         <v>41883</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D194" s="3">
         <v>-44.4444444444444</v>
@@ -5166,10 +5247,10 @@
         <v>41883</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D195" s="3">
         <v>-44.4444444444444</v>
@@ -5186,10 +5267,10 @@
         <v>41883</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D196" s="3">
         <v>-44.4444444444444</v>
@@ -5206,10 +5287,10 @@
         <v>41883</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D197" s="3">
         <v>-44.4444444444444</v>
@@ -5226,10 +5307,10 @@
         <v>41883</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D198" s="3">
         <v>-44.4444444444444</v>
@@ -5246,10 +5327,10 @@
         <v>41883</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D199" s="3">
         <v>-44.4444444444444</v>
@@ -5266,10 +5347,10 @@
         <v>41883</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D200" s="3">
         <v>-44.4444444444444</v>
@@ -5286,10 +5367,10 @@
         <v>41883</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D201" s="3">
         <v>-44.4444444444444</v>
@@ -5306,19 +5387,19 @@
         <v>41883</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="D202" s="3">
-        <v>-618.515555555556</v>
+        <v>-44.4444444444444</v>
       </c>
       <c r="E202" s="3">
         <v>0</v>
       </c>
       <c r="F202" s="3">
-        <v>-618.515555555556</v>
+        <v>-44.4444444444444</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -5326,19 +5407,19 @@
         <v>41883</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D203" s="3">
-        <v>-815.946666666667</v>
+        <v>-618.515555555556</v>
       </c>
       <c r="E203" s="3">
         <v>0</v>
       </c>
       <c r="F203" s="3">
-        <v>-815.946666666667</v>
+        <v>-618.515555555556</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -5346,19 +5427,19 @@
         <v>41883</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="D204" s="3">
-        <v>-1739.28888888889</v>
+        <v>-815.946666666667</v>
       </c>
       <c r="E204" s="3">
         <v>0</v>
       </c>
       <c r="F204" s="3">
-        <v>-1739.28888888889</v>
+        <v>-815.946666666667</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -5366,19 +5447,19 @@
         <v>41883</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D205" s="3">
-        <v>-2498.88888888889</v>
+        <v>-1739.28888888889</v>
       </c>
       <c r="E205" s="3">
         <v>0</v>
       </c>
       <c r="F205" s="3">
-        <v>-2498.88888888889</v>
+        <v>-1739.28888888889</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -5386,19 +5467,19 @@
         <v>41883</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="D206" s="3">
-        <v>-618.888888888889</v>
+        <v>-2498.88888888889</v>
       </c>
       <c r="E206" s="3">
         <v>0</v>
       </c>
       <c r="F206" s="3">
-        <v>-618.888888888889</v>
+        <v>-2498.88888888889</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -5406,19 +5487,19 @@
         <v>41883</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D207" s="3">
-        <v>-850.22</v>
+        <v>-618.888888888889</v>
       </c>
       <c r="E207" s="3">
         <v>0</v>
       </c>
       <c r="F207" s="3">
-        <v>-850.22</v>
+        <v>-618.888888888889</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -5426,19 +5507,19 @@
         <v>41883</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D208" s="3">
-        <v>-578.071111111111</v>
+        <v>-850.22</v>
       </c>
       <c r="E208" s="3">
         <v>0</v>
       </c>
       <c r="F208" s="3">
-        <v>-578.071111111111</v>
+        <v>-850.22</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -5446,19 +5527,19 @@
         <v>41883</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="D209" s="3">
-        <v>-1289.2</v>
+        <v>-578.071111111111</v>
       </c>
       <c r="E209" s="3">
         <v>0</v>
       </c>
       <c r="F209" s="3">
-        <v>-1289.2</v>
+        <v>-578.071111111111</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -5466,19 +5547,19 @@
         <v>41883</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="D210" s="3">
-        <v>-729.626666666667</v>
+        <v>-1289.2</v>
       </c>
       <c r="E210" s="3">
         <v>0</v>
       </c>
       <c r="F210" s="3">
-        <v>-729.626666666667</v>
+        <v>-1289.2</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -5486,19 +5567,19 @@
         <v>41883</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="D211" s="3">
-        <v>-683.848888888889</v>
+        <v>-729.626666666667</v>
       </c>
       <c r="E211" s="3">
         <v>0</v>
       </c>
       <c r="F211" s="3">
-        <v>-683.848888888889</v>
+        <v>-729.626666666667</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -5506,39 +5587,39 @@
         <v>41883</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="D212" s="3">
-        <v>-2138.97777777778</v>
+        <v>-683.848888888889</v>
       </c>
       <c r="E212" s="3">
         <v>0</v>
       </c>
       <c r="F212" s="3">
-        <v>-2138.97777777778</v>
+        <v>-683.848888888889</v>
       </c>
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="2">
-        <v>41913</v>
+        <v>41883</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="D213" s="3">
-        <v>-1196.83673469388</v>
+        <v>-2138.97777777778</v>
       </c>
       <c r="E213" s="3">
         <v>0</v>
       </c>
       <c r="F213" s="3">
-        <v>-1196.83673469388</v>
+        <v>-2138.97777777778</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -5546,19 +5627,19 @@
         <v>41913</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="D214" s="3">
-        <v>-332.755102040816</v>
+        <v>-1196.83673469388</v>
       </c>
       <c r="E214" s="3">
         <v>0</v>
       </c>
       <c r="F214" s="3">
-        <v>-332.755102040816</v>
+        <v>-1196.83673469388</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -5566,19 +5647,19 @@
         <v>41913</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="D215" s="3">
-        <v>-1980.9</v>
+        <v>-332.755102040816</v>
       </c>
       <c r="E215" s="3">
-        <v>-34.98</v>
+        <v>0</v>
       </c>
       <c r="F215" s="3">
-        <v>-2015.88</v>
+        <v>-332.755102040816</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -5586,19 +5667,19 @@
         <v>41913</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="D216" s="3">
-        <v>-882.040816326531</v>
+        <v>-1980.9</v>
       </c>
       <c r="E216" s="3">
-        <v>0</v>
+        <v>-34.98</v>
       </c>
       <c r="F216" s="3">
-        <v>-882.040816326531</v>
+        <v>-2015.88</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -5606,19 +5687,19 @@
         <v>41913</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="D217" s="3">
-        <v>-937.408163265306</v>
+        <v>-882.040816326531</v>
       </c>
       <c r="E217" s="3">
         <v>0</v>
       </c>
       <c r="F217" s="3">
-        <v>-937.408163265306</v>
+        <v>-882.040816326531</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -5626,19 +5707,19 @@
         <v>41913</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="D218" s="3">
-        <v>-1226.88</v>
+        <v>-937.408163265306</v>
       </c>
       <c r="E218" s="3">
         <v>0</v>
       </c>
       <c r="F218" s="3">
-        <v>-1226.88</v>
+        <v>-937.408163265306</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -5646,19 +5727,19 @@
         <v>41913</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="D219" s="3">
-        <v>-1077.24489795918</v>
+        <v>-1226.88</v>
       </c>
       <c r="E219" s="3">
         <v>0</v>
       </c>
       <c r="F219" s="3">
-        <v>-1077.24489795918</v>
+        <v>-1226.88</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -5666,19 +5747,19 @@
         <v>41913</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D220" s="3">
-        <v>-734.69387755102</v>
+        <v>-1077.24489795918</v>
       </c>
       <c r="E220" s="3">
         <v>0</v>
       </c>
       <c r="F220" s="3">
-        <v>-734.69387755102</v>
+        <v>-1077.24489795918</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -5686,19 +5767,19 @@
         <v>41913</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="D221" s="3">
-        <v>0</v>
+        <v>-734.69387755102</v>
       </c>
       <c r="E221" s="3">
-        <v>-35</v>
+        <v>0</v>
       </c>
       <c r="F221" s="3">
-        <v>-35</v>
+        <v>-734.69387755102</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -5706,19 +5787,19 @@
         <v>41913</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="D222" s="3">
-        <v>-1522.04081632653</v>
+        <v>0</v>
       </c>
       <c r="E222" s="3">
-        <v>0</v>
+        <v>-35</v>
       </c>
       <c r="F222" s="3">
-        <v>-1522.04081632653</v>
+        <v>-35</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -5726,19 +5807,19 @@
         <v>41913</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D223" s="3">
-        <v>-832.877551020408</v>
+        <v>-1522.04081632653</v>
       </c>
       <c r="E223" s="3">
         <v>0</v>
       </c>
       <c r="F223" s="3">
-        <v>-832.877551020408</v>
+        <v>-1522.04081632653</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -5746,19 +5827,19 @@
         <v>41913</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="D224" s="3">
-        <v>-1099.69387755102</v>
+        <v>-832.877551020408</v>
       </c>
       <c r="E224" s="3">
         <v>0</v>
       </c>
       <c r="F224" s="3">
-        <v>-1099.69387755102</v>
+        <v>-832.877551020408</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -5766,19 +5847,19 @@
         <v>41913</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="D225" s="3">
-        <v>-371.938775510204</v>
+        <v>-1099.69387755102</v>
       </c>
       <c r="E225" s="3">
         <v>0</v>
       </c>
       <c r="F225" s="3">
-        <v>-371.938775510204</v>
+        <v>-1099.69387755102</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -5786,19 +5867,19 @@
         <v>41913</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>279</v>
+        <v>318</v>
       </c>
       <c r="D226" s="3">
-        <v>-566.938775510204</v>
+        <v>-371.938775510204</v>
       </c>
       <c r="E226" s="3">
         <v>0</v>
       </c>
       <c r="F226" s="3">
-        <v>-566.938775510204</v>
+        <v>-371.938775510204</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -5806,19 +5887,19 @@
         <v>41913</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D227" s="3">
-        <v>-731.942857142857</v>
+        <v>-566.938775510204</v>
       </c>
       <c r="E227" s="3">
         <v>0</v>
       </c>
       <c r="F227" s="3">
-        <v>-731.942857142857</v>
+        <v>-566.938775510204</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -5826,19 +5907,19 @@
         <v>41913</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="D228" s="3">
-        <v>-1041.32653061224</v>
+        <v>-731.942857142857</v>
       </c>
       <c r="E228" s="3">
         <v>0</v>
       </c>
       <c r="F228" s="3">
-        <v>-1041.32653061224</v>
+        <v>-731.942857142857</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -5846,19 +5927,19 @@
         <v>41913</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="D229" s="3">
-        <v>-283.469387755102</v>
+        <v>-1041.32653061224</v>
       </c>
       <c r="E229" s="3">
         <v>0</v>
       </c>
       <c r="F229" s="3">
-        <v>-283.469387755102</v>
+        <v>-1041.32653061224</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -5866,19 +5947,19 @@
         <v>41913</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>225</v>
+        <v>174</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D230" s="3">
-        <v>-369.489795918367</v>
+        <v>-283.469387755102</v>
       </c>
       <c r="E230" s="3">
         <v>0</v>
       </c>
       <c r="F230" s="3">
-        <v>-369.489795918367</v>
+        <v>-283.469387755102</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -5886,19 +5967,19 @@
         <v>41913</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="D231" s="3">
-        <v>-1169.08163265306</v>
+        <v>-369.489795918367</v>
       </c>
       <c r="E231" s="3">
         <v>0</v>
       </c>
       <c r="F231" s="3">
-        <v>-1169.08163265306</v>
+        <v>-369.489795918367</v>
       </c>
     </row>
     <row r="232" spans="1:6">
@@ -5906,19 +5987,19 @@
         <v>41913</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="D232" s="3">
-        <v>-209.387755102041</v>
+        <v>-1169.08163265306</v>
       </c>
       <c r="E232" s="3">
         <v>0</v>
       </c>
       <c r="F232" s="3">
-        <v>-209.387755102041</v>
+        <v>-1169.08163265306</v>
       </c>
     </row>
     <row r="233" spans="1:6">
@@ -5929,7 +6010,7 @@
         <v>227</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D233" s="3">
         <v>-209.387755102041</v>
@@ -5946,39 +6027,39 @@
         <v>41913</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="D234" s="3">
-        <v>-1256.95510204082</v>
+        <v>-209.387755102041</v>
       </c>
       <c r="E234" s="3">
         <v>0</v>
       </c>
       <c r="F234" s="3">
-        <v>-1256.95510204082</v>
+        <v>-209.387755102041</v>
       </c>
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="2">
-        <v>41944</v>
+        <v>41913</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="D235" s="3">
-        <v>-409.12</v>
+        <v>-1256.95510204082</v>
       </c>
       <c r="E235" s="3">
         <v>0</v>
       </c>
       <c r="F235" s="3">
-        <v>-409.12</v>
+        <v>-1256.95510204082</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -5986,19 +6067,19 @@
         <v>41944</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="D236" s="3">
-        <v>-360</v>
+        <v>-409.12</v>
       </c>
       <c r="E236" s="3">
         <v>0</v>
       </c>
       <c r="F236" s="3">
-        <v>-360</v>
+        <v>-409.12</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -6006,19 +6087,19 @@
         <v>41944</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>279</v>
+        <v>314</v>
       </c>
       <c r="D237" s="3">
-        <v>-555.6</v>
+        <v>-361.864</v>
       </c>
       <c r="E237" s="3">
         <v>0</v>
       </c>
       <c r="F237" s="3">
-        <v>-555.6</v>
+        <v>-361.864</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -6026,19 +6107,19 @@
         <v>41944</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D238" s="3">
-        <v>-1478.2</v>
+        <v>-555.6</v>
       </c>
       <c r="E238" s="3">
         <v>0</v>
       </c>
       <c r="F238" s="3">
-        <v>-1478.2</v>
+        <v>-555.6</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -6046,19 +6127,19 @@
         <v>41944</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="D239" s="3">
-        <v>-555.6</v>
+        <v>-1490.8</v>
       </c>
       <c r="E239" s="3">
         <v>0</v>
       </c>
       <c r="F239" s="3">
-        <v>-555.6</v>
+        <v>-1490.8</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -6066,19 +6147,19 @@
         <v>41944</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D240" s="3">
-        <v>-408</v>
+        <v>-555.6</v>
       </c>
       <c r="E240" s="3">
         <v>0</v>
       </c>
       <c r="F240" s="3">
-        <v>-408</v>
+        <v>-555.6</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -6086,19 +6167,19 @@
         <v>41944</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="D241" s="3">
-        <v>-360</v>
+        <v>-408</v>
       </c>
       <c r="E241" s="3">
         <v>0</v>
       </c>
       <c r="F241" s="3">
-        <v>-360</v>
+        <v>-408</v>
       </c>
     </row>
     <row r="242" spans="1:6">
@@ -6106,19 +6187,19 @@
         <v>41944</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>290</v>
+        <v>320</v>
       </c>
       <c r="D242" s="3">
-        <v>-435.12</v>
+        <v>-361.864</v>
       </c>
       <c r="E242" s="3">
         <v>0</v>
       </c>
       <c r="F242" s="3">
-        <v>-435.12</v>
+        <v>-361.864</v>
       </c>
     </row>
     <row r="243" spans="1:6">
@@ -6126,19 +6207,19 @@
         <v>41944</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D243" s="3">
-        <v>-410.1</v>
+        <v>-435.12</v>
       </c>
       <c r="E243" s="3">
         <v>0</v>
       </c>
       <c r="F243" s="3">
-        <v>-410.1</v>
+        <v>-435.12</v>
       </c>
     </row>
     <row r="244" spans="1:6">
@@ -6146,19 +6227,19 @@
         <v>41944</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>279</v>
+        <v>319</v>
       </c>
       <c r="D244" s="3">
-        <v>-555.6</v>
+        <v>-410.1</v>
       </c>
       <c r="E244" s="3">
         <v>0</v>
       </c>
       <c r="F244" s="3">
-        <v>-555.6</v>
+        <v>-410.1</v>
       </c>
     </row>
     <row r="245" spans="1:6">
@@ -6166,19 +6247,19 @@
         <v>41944</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D245" s="3">
-        <v>-1554.048</v>
+        <v>-555.6</v>
       </c>
       <c r="E245" s="3">
         <v>0</v>
       </c>
       <c r="F245" s="3">
-        <v>-1554.048</v>
+        <v>-555.6</v>
       </c>
     </row>
     <row r="246" spans="1:6">
@@ -6186,19 +6267,19 @@
         <v>41944</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>278</v>
+        <v>307</v>
       </c>
       <c r="D246" s="3">
-        <v>-216</v>
+        <v>-1557.548</v>
       </c>
       <c r="E246" s="3">
         <v>0</v>
       </c>
       <c r="F246" s="3">
-        <v>-216</v>
+        <v>-1557.548</v>
       </c>
     </row>
     <row r="247" spans="1:6">
@@ -6206,19 +6287,19 @@
         <v>41944</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="D247" s="3">
-        <v>-360</v>
+        <v>-365.2</v>
       </c>
       <c r="E247" s="3">
         <v>0</v>
       </c>
       <c r="F247" s="3">
-        <v>-360</v>
+        <v>-365.2</v>
       </c>
     </row>
     <row r="248" spans="1:6">
@@ -6229,7 +6310,7 @@
         <v>107</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="D248" s="3">
         <v>-168</v>
@@ -6246,10 +6327,10 @@
         <v>41944</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="D249" s="3">
         <v>-408</v>
@@ -6266,10 +6347,10 @@
         <v>41944</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D250" s="3">
         <v>-555.6</v>
@@ -6286,10 +6367,10 @@
         <v>41944</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>278</v>
+        <v>322</v>
       </c>
       <c r="D251" s="3">
         <v>-640</v>
@@ -6306,10 +6387,10 @@
         <v>41944</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="D252" s="3">
         <v>-1904.848</v>
@@ -6326,19 +6407,19 @@
         <v>41944</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D253" s="3">
-        <v>-408</v>
+        <v>-409.864</v>
       </c>
       <c r="E253" s="3">
         <v>0</v>
       </c>
       <c r="F253" s="3">
-        <v>-408</v>
+        <v>-409.864</v>
       </c>
     </row>
     <row r="254" spans="1:6">
@@ -6346,19 +6427,19 @@
         <v>41944</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="D254" s="3">
-        <v>-1807.6</v>
+        <v>-1824.4</v>
       </c>
       <c r="E254" s="3">
         <v>0</v>
       </c>
       <c r="F254" s="3">
-        <v>-1807.6</v>
+        <v>-1824.4</v>
       </c>
     </row>
     <row r="255" spans="1:6">
@@ -6366,19 +6447,19 @@
         <v>41944</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D255" s="3">
-        <v>-1447.2</v>
+        <v>-1449.3</v>
       </c>
       <c r="E255" s="3">
         <v>0</v>
       </c>
       <c r="F255" s="3">
-        <v>-1447.2</v>
+        <v>-1449.3</v>
       </c>
     </row>
     <row r="256" spans="1:6">
@@ -6386,10 +6467,10 @@
         <v>41944</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D256" s="3">
         <v>-555.6</v>
@@ -6406,19 +6487,19 @@
         <v>41944</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="D257" s="3">
-        <v>-408</v>
+        <v>-409.864</v>
       </c>
       <c r="E257" s="3">
         <v>0</v>
       </c>
       <c r="F257" s="3">
-        <v>-408</v>
+        <v>-409.864</v>
       </c>
     </row>
     <row r="258" spans="1:6">
@@ -6426,19 +6507,19 @@
         <v>41944</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="D258" s="3">
-        <v>-360</v>
+        <v>-361.12</v>
       </c>
       <c r="E258" s="3">
         <v>0</v>
       </c>
       <c r="F258" s="3">
-        <v>-360</v>
+        <v>-361.12</v>
       </c>
     </row>
     <row r="259" spans="1:6">
@@ -6446,19 +6527,19 @@
         <v>41944</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D259" s="3">
-        <v>-508</v>
+        <v>-520.264</v>
       </c>
       <c r="E259" s="3">
         <v>0</v>
       </c>
       <c r="F259" s="3">
-        <v>-508</v>
+        <v>-520.264</v>
       </c>
     </row>
     <row r="260" spans="1:6">
@@ -6466,10 +6547,10 @@
         <v>41944</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="D260" s="3">
         <v>-360</v>
@@ -6486,19 +6567,19 @@
         <v>41944</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D261" s="3">
-        <v>-1431.2</v>
+        <v>-1448</v>
       </c>
       <c r="E261" s="3">
         <v>0</v>
       </c>
       <c r="F261" s="3">
-        <v>-1431.2</v>
+        <v>-1448</v>
       </c>
     </row>
     <row r="262" spans="1:6">
@@ -6506,10 +6587,10 @@
         <v>41944</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D262" s="3">
         <v>-1628.8</v>
@@ -6526,10 +6607,10 @@
         <v>41974</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D263" s="3">
         <v>-762.645914396887</v>
@@ -6546,10 +6627,10 @@
         <v>41974</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="D264" s="3">
         <v>-256.809338521401</v>
@@ -6566,10 +6647,10 @@
         <v>41974</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D265" s="3">
         <v>-540.466926070039</v>
@@ -6586,19 +6667,19 @@
         <v>41974</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D266" s="3">
-        <v>-540.466926070039</v>
+        <v>-541.828793774319</v>
       </c>
       <c r="E266" s="3">
         <v>0</v>
       </c>
       <c r="F266" s="3">
-        <v>-540.466926070039</v>
+        <v>-541.828793774319</v>
       </c>
     </row>
     <row r="267" spans="1:6">
@@ -6606,10 +6687,10 @@
         <v>41974</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
       <c r="D267" s="3">
         <v>-1244.94163424125</v>
@@ -6626,19 +6707,19 @@
         <v>41974</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>278</v>
+        <v>324</v>
       </c>
       <c r="D268" s="3">
-        <v>-350.194552529183</v>
+        <v>-351.284046692607</v>
       </c>
       <c r="E268" s="3">
         <v>0</v>
       </c>
       <c r="F268" s="3">
-        <v>-350.194552529183</v>
+        <v>-351.284046692607</v>
       </c>
     </row>
     <row r="269" spans="1:6">
@@ -6646,10 +6727,10 @@
         <v>41974</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D269" s="3">
         <v>-247.081712062257</v>
@@ -6666,10 +6747,10 @@
         <v>41974</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D270" s="3">
         <v>-247.081712062257</v>
@@ -6686,10 +6767,10 @@
         <v>41974</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D271" s="3">
         <v>-247.081712062257</v>
@@ -6706,10 +6787,10 @@
         <v>41974</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D272" s="3">
         <v>-247.081712062257</v>
@@ -6726,10 +6807,10 @@
         <v>41974</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D273" s="3">
         <v>-1069.64980544747</v>
@@ -6746,10 +6827,10 @@
         <v>41974</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="D274" s="3">
         <v>-769.416342412451</v>
@@ -6766,10 +6847,10 @@
         <v>41974</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="D275" s="3">
         <v>-540.466926070039</v>
@@ -6786,10 +6867,10 @@
         <v>41974</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D276" s="3">
         <v>-1563.81322957198</v>
@@ -6806,10 +6887,10 @@
         <v>41974</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D277" s="3">
         <v>-1036.18677042802</v>
@@ -6826,10 +6907,10 @@
         <v>41974</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="D278" s="3">
         <v>-661.47859922179</v>
@@ -6846,10 +6927,10 @@
         <v>41974</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D279" s="3">
         <v>-821.011673151751</v>
@@ -6866,19 +6947,19 @@
         <v>42005</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D280" s="3">
-        <v>-1475.48638132296</v>
+        <v>-1480.93385214008</v>
       </c>
       <c r="E280" s="3">
         <v>0</v>
       </c>
       <c r="F280" s="3">
-        <v>-1475.48638132296</v>
+        <v>-1480.93385214008</v>
       </c>
     </row>
     <row r="281" spans="1:6">
@@ -6886,19 +6967,19 @@
         <v>42005</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D281" s="3">
-        <v>-1580.93385214008</v>
+        <v>-1591.82879377432</v>
       </c>
       <c r="E281" s="3">
         <v>0</v>
       </c>
       <c r="F281" s="3">
-        <v>-1580.93385214008</v>
+        <v>-1591.82879377432</v>
       </c>
     </row>
     <row r="282" spans="1:6">
@@ -6906,10 +6987,10 @@
         <v>42005</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D282" s="3">
         <v>-566.938775510204</v>
@@ -6926,10 +7007,10 @@
         <v>42005</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D283" s="3">
         <v>-540.466926070039</v>
@@ -6946,10 +7027,10 @@
         <v>42005</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D284" s="3">
         <v>-500</v>
@@ -6966,19 +7047,19 @@
         <v>42005</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D285" s="3">
-        <v>-1577.43190661479</v>
+        <v>-1582.87937743191</v>
       </c>
       <c r="E285" s="3">
         <v>0</v>
       </c>
       <c r="F285" s="3">
-        <v>-1577.43190661479</v>
+        <v>-1582.87937743191</v>
       </c>
     </row>
     <row r="286" spans="1:6">
@@ -6986,10 +7067,10 @@
         <v>42005</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="D286" s="3">
         <v>-198.443579766537</v>
@@ -7000,6 +7081,118 @@
       <c r="F286" s="3">
         <v>-198.443579766537</v>
       </c>
+    </row>
+    <row r="287" spans="1:6">
+      <c r="A287" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D287" s="3"/>
+      <c r="E287" s="3">
+        <v>0</v>
+      </c>
+      <c r="F287" s="3"/>
+    </row>
+    <row r="288" spans="1:6">
+      <c r="A288" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D288" s="3"/>
+      <c r="E288" s="3">
+        <v>0</v>
+      </c>
+      <c r="F288" s="3"/>
+    </row>
+    <row r="289" spans="1:6">
+      <c r="A289" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D289" s="3"/>
+      <c r="E289" s="3">
+        <v>0</v>
+      </c>
+      <c r="F289" s="3"/>
+    </row>
+    <row r="290" spans="1:6">
+      <c r="A290" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D290" s="3"/>
+      <c r="E290" s="3">
+        <v>0</v>
+      </c>
+      <c r="F290" s="3"/>
+    </row>
+    <row r="291" spans="1:6">
+      <c r="A291" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D291" s="3"/>
+      <c r="E291" s="3">
+        <v>0</v>
+      </c>
+      <c r="F291" s="3"/>
+    </row>
+    <row r="292" spans="1:6">
+      <c r="A292" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D292" s="3"/>
+      <c r="E292" s="3">
+        <v>0</v>
+      </c>
+      <c r="F292" s="3"/>
+    </row>
+    <row r="293" spans="1:6">
+      <c r="A293" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D293" s="3"/>
+      <c r="E293" s="3">
+        <v>0</v>
+      </c>
+      <c r="F293" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>